<commit_message>
Update RacingTeam.zip, PCBBom.xlsx, and 2 more files...
</commit_message>
<xml_diff>
--- a/RacingTeam/PCBBom.xlsx
+++ b/RacingTeam/PCBBom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayden Bourdeau\SyncedGit\RacingTeam\RacingTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9325E39-C2FD-4F7A-8B16-722264927A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7710C6A-4D32-445C-812A-DAF91055C035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10815" yWindow="1095" windowWidth="21600" windowHeight="11385" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
+    <workbookView xWindow="0" yWindow="1095" windowWidth="21600" windowHeight="11385" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Item</t>
   </si>
@@ -196,6 +196,153 @@
   </si>
   <si>
     <t>2034-1106-ND</t>
+  </si>
+  <si>
+    <t>R1-R4</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805FT249K/1760185</t>
+  </si>
+  <si>
+    <t>Resistor for Voltage Division (249k) (0805)</t>
+  </si>
+  <si>
+    <t>RMCF0805FT249K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RNCP0805FTD1K30/2240232</t>
+  </si>
+  <si>
+    <t>Resistor for Voltage Division (1.3k) (0805)</t>
+  </si>
+  <si>
+    <t>R7-R9</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD1K30</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/rohm-semiconductor/ESR03EZPJ101/1983452</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ101</t>
+  </si>
+  <si>
+    <t>Resistor for Input Op Amp (100ohm) (0603)</t>
+  </si>
+  <si>
+    <t>Resistors for CMOS Pullup (22k) (0805)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/te-connectivity-passive-product/CRG0805F22K/2380871</t>
+  </si>
+  <si>
+    <t>CRG0805F22K</t>
+  </si>
+  <si>
+    <t>Resistor for Opto</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>CRGCQ0603F1K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/te-connectivity-passive-product/CRGCQ0603F1K2/8576291</t>
+  </si>
+  <si>
+    <t>Resistor for CMOS Pullup</t>
+  </si>
+  <si>
+    <t>R14,R19</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RNCP0603FTD10K0/2240139</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0</t>
+  </si>
+  <si>
+    <t>XZM2CRK54WA-8</t>
+  </si>
+  <si>
+    <t>Diagnostic LED's (Red)</t>
+  </si>
+  <si>
+    <t>Diagnostic LED's (Green)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sunled/XZM2CRK54WA-8/8571166</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERA-3AEB4990V/2026721</t>
+  </si>
+  <si>
+    <t>ERA-3AEB4990V</t>
+  </si>
+  <si>
+    <t>Resistor for LED (499Ohm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sunled/XZVG54W-8/8259041</t>
+  </si>
+  <si>
+    <t>XZVG54W-8</t>
+  </si>
+  <si>
+    <t>Resistor for Voltage Division(150k) (0805)</t>
+  </si>
+  <si>
+    <t>ERJ-P06J154V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERJ-P06J154V/525220</t>
+  </si>
+  <si>
+    <t>RT0805FRE074K02L</t>
+  </si>
+  <si>
+    <t>Resistor for Voltage Division(4020) (0805)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RT0805FRE074K02L/1079285</t>
+  </si>
+  <si>
+    <t>R18,R20</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>R12, R15,R16,R17,R29</t>
+  </si>
+  <si>
+    <t>R10,R11, R27, R28</t>
+  </si>
+  <si>
+    <t>Resistor for Voltage Division (4.7k) (0805)</t>
+  </si>
+  <si>
+    <t>Resistor for Voltage Division (6.8k) (0805)</t>
+  </si>
+  <si>
+    <t>CRGCQ0805J4K7</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/te-connectivity-passive-product/CRGCQ0805J4K7/8576740</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/walsin-technology-corporation/WR08X6801FTL/13238733</t>
+  </si>
+  <si>
+    <t>WR08X6801FTL</t>
+  </si>
+  <si>
+    <t>Resistor for Relays (Non Connected) (0603)</t>
   </si>
 </sst>
 </file>
@@ -566,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659DCB98-9E00-43BC-A3B3-A9EBD8392DA4}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +908,7 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2">
-        <f t="shared" ref="K9:K25" si="0">G9*I9</f>
+        <f t="shared" ref="K9:K26" si="0">G9*I9</f>
         <v>0.63</v>
       </c>
       <c r="L9" s="2"/>
@@ -974,189 +1121,380 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2">
+        <v>0.15</v>
+      </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="I17" s="2">
+        <v>4</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2">
+        <v>0.15</v>
+      </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="I18" s="2">
+        <v>3</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2">
+        <v>0.15</v>
+      </c>
       <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="M19" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2">
+        <v>0.15</v>
+      </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="2">
+        <v>5</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <v>0.15</v>
+      </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="M21" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>0.15</v>
+      </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
+      <c r="M22" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2">
+        <v>0.51</v>
+      </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="M23" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2">
+        <v>0.84</v>
+      </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
+      <c r="M24" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2">
+        <v>0.69</v>
+      </c>
       <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
+      <c r="M25" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2">
+        <v>0.19</v>
+      </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="I26" s="2">
+        <v>3</v>
+      </c>
       <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="K26" s="2">
+        <f>I26*G26</f>
+        <v>0.57000000000000006</v>
+      </c>
       <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
+      <c r="M26" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <f>I27*G27</f>
+        <v>0.15</v>
+      </c>
+      <c r="M27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f>G28*I28</f>
+        <v>0.15</v>
+      </c>
+      <c r="M28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <f>G29*I29</f>
+        <v>0.15</v>
+      </c>
+      <c r="M29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M6" r:id="rId1" xr:uid="{CEEC209E-8376-4C35-8907-FCE312106A71}"/>
     <hyperlink ref="M7" r:id="rId2" xr:uid="{08492305-3068-40B0-ACFA-C33610E51BF3}"/>
     <hyperlink ref="M16" r:id="rId3" xr:uid="{0A338AD5-2390-4296-A72F-5743302DA168}"/>
+    <hyperlink ref="M19" r:id="rId4" xr:uid="{7E7D32F3-55C9-41D4-86D5-2057C2673203}"/>
+    <hyperlink ref="M5" r:id="rId5" xr:uid="{51E2BD66-0F1C-48A9-B25C-67F1EB183828}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 2N7002H6327XTSA2.kicad_mod, 4N35SM.kicad_mod, and 21 more files...
</commit_message>
<xml_diff>
--- a/RacingTeam/PCBBom.xlsx
+++ b/RacingTeam/PCBBom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayden Bourdeau\SyncedGit\RacingTeam\RacingTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7710C6A-4D32-445C-812A-DAF91055C035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817C11C2-F8F9-4858-A5CF-C6C79A970307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1095" windowWidth="21600" windowHeight="11385" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
+    <workbookView xWindow="24585" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Item</t>
   </si>
@@ -159,12 +159,6 @@
     <t>https://www.digikey.ca/en/products/detail/texas-instruments/NE555PSRE4/1571968</t>
   </si>
   <si>
-    <t>BSS138W</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/diodes-incorporated/BSS138W-7-F/814992?utm_campaign=buynow&amp;utm_medium=aggregator&amp;WT.z_cid=ref_findchips_standard&amp;utm_source=findchips</t>
-  </si>
-  <si>
     <t>CPH6350-TL-W</t>
   </si>
   <si>
@@ -342,7 +336,16 @@
     <t>WR08X6801FTL</t>
   </si>
   <si>
-    <t>Resistor for Relays (Non Connected) (0603)</t>
+    <t>Resistor for Relays (Non Connected) (0603) (700ohm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/infineon-technologies/2N7002H6327XTSA2/5410097</t>
+  </si>
+  <si>
+    <t>2N7002H6327XTSA2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0603FT732R/1714224</t>
   </si>
 </sst>
 </file>
@@ -393,11 +396,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -715,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659DCB98-9E00-43BC-A3B3-A9EBD8392DA4}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,11 +776,11 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
@@ -793,7 +797,7 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="3" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -802,11 +806,11 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
@@ -882,7 +886,7 @@
         <v>2.39</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -908,11 +912,11 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2">
-        <f t="shared" ref="K9:K26" si="0">G9*I9</f>
+        <f t="shared" ref="K9:K25" si="0">G9*I9</f>
         <v>0.63</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -936,7 +940,7 @@
         <f>G10*I10</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -966,7 +970,7 @@
         <v>3.3000000000000003</v>
       </c>
       <c r="L11" s="2"/>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -996,7 +1000,7 @@
         <v>3.14</v>
       </c>
       <c r="L12" s="2"/>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1026,7 +1030,7 @@
         <v>1.17</v>
       </c>
       <c r="L13" s="2"/>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1056,21 +1060,21 @@
         <v>0.18</v>
       </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
@@ -1086,21 +1090,21 @@
         <v>1.9500000000000002</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="2" t="s">
-        <v>46</v>
+      <c r="M15" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
@@ -1117,20 +1121,20 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
@@ -1147,20 +1151,20 @@
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
@@ -1177,20 +1181,20 @@
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
@@ -1207,20 +1211,20 @@
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
@@ -1237,20 +1241,20 @@
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
@@ -1267,20 +1271,20 @@
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
@@ -1297,20 +1301,20 @@
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
@@ -1327,20 +1331,20 @@
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
@@ -1356,21 +1360,21 @@
         <v>0.84</v>
       </c>
       <c r="L24" s="2"/>
-      <c r="M24" s="2" t="s">
-        <v>79</v>
+      <c r="M24" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
@@ -1386,19 +1390,19 @@
         <v>0.69</v>
       </c>
       <c r="L25" s="2"/>
-      <c r="M25" s="2" t="s">
-        <v>83</v>
+      <c r="M25" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
@@ -1415,15 +1419,15 @@
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G27" s="2">
         <v>0.15</v>
@@ -1436,15 +1440,15 @@
         <v>0.15</v>
       </c>
       <c r="M27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
         <v>96</v>
-      </c>
-      <c r="E28" t="s">
-        <v>98</v>
       </c>
       <c r="G28" s="2">
         <v>0.15</v>
@@ -1457,15 +1461,15 @@
         <v>0.15</v>
       </c>
       <c r="M28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G29" s="2">
         <v>0.15</v>
@@ -1478,12 +1482,25 @@
         <v>0.15</v>
       </c>
       <c r="M29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I30" s="2">
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <f>G30*I30</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="M30" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1492,9 +1509,19 @@
     <hyperlink ref="M7" r:id="rId2" xr:uid="{08492305-3068-40B0-ACFA-C33610E51BF3}"/>
     <hyperlink ref="M16" r:id="rId3" xr:uid="{0A338AD5-2390-4296-A72F-5743302DA168}"/>
     <hyperlink ref="M19" r:id="rId4" xr:uid="{7E7D32F3-55C9-41D4-86D5-2057C2673203}"/>
-    <hyperlink ref="M5" r:id="rId5" xr:uid="{51E2BD66-0F1C-48A9-B25C-67F1EB183828}"/>
+    <hyperlink ref="M25" r:id="rId5" xr:uid="{E4C7D041-3439-4529-8781-C56520BD1941}"/>
+    <hyperlink ref="M24" r:id="rId6" xr:uid="{59A75E64-76BD-4F26-9038-998CD8C64ED1}"/>
+    <hyperlink ref="M15" r:id="rId7" xr:uid="{2AFFE17E-B2EF-458B-B31F-F4CC139887F1}"/>
+    <hyperlink ref="M14" r:id="rId8" xr:uid="{2FBA0AE0-F035-4237-9D60-353C0F54C66F}"/>
+    <hyperlink ref="M13" r:id="rId9" xr:uid="{A6FFBE5B-1F72-448E-B1C1-843B0A30946E}"/>
+    <hyperlink ref="M12" r:id="rId10" xr:uid="{F623AF18-E7D9-477F-8361-17BAB023C529}"/>
+    <hyperlink ref="M11" r:id="rId11" xr:uid="{746B69B6-384E-4501-8621-737CF897D979}"/>
+    <hyperlink ref="M10" r:id="rId12" xr:uid="{152BFDF8-F03E-40E6-AB3A-FBC1FD093250}"/>
+    <hyperlink ref="M9" r:id="rId13" xr:uid="{2E109D78-6982-4043-8D6D-48296465E121}"/>
+    <hyperlink ref="M8" r:id="rId14" xr:uid="{D063395C-1335-4145-9AAE-EBBC5462897E}"/>
+    <hyperlink ref="M5" r:id="rId15" xr:uid="{073FF774-A8B3-4EB6-865F-37A44A0EE3EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update FUSE_0154004.DRTL.kicad_mod, GRC2022.mod, and 15 more files...
</commit_message>
<xml_diff>
--- a/RacingTeam/PCBBom.xlsx
+++ b/RacingTeam/PCBBom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayden Bourdeau\SyncedGit\RacingTeam\RacingTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817C11C2-F8F9-4858-A5CF-C6C79A970307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216B1598-B2C7-407D-A471-616F261AD15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24585" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>Item</t>
   </si>
@@ -346,6 +346,18 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0603FT732R/1714224</t>
+  </si>
+  <si>
+    <t>Fuse Holder SMD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/littelfuse-inc/0154003-DR/183356</t>
+  </si>
+  <si>
+    <t>Fuse 2-SMD</t>
+  </si>
+  <si>
+    <t>F1-F5</t>
   </si>
 </sst>
 </file>
@@ -717,9 +729,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659DCB98-9E00-43BC-A3B3-A9EBD8392DA4}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1501,6 +1513,35 @@
       </c>
       <c r="M30" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="2">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="I31" s="2">
+        <v>5</v>
+      </c>
+      <c r="K31">
+        <f>I31*G31</f>
+        <v>20.299999999999997</v>
+      </c>
+      <c r="M31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update PCBBom.xlsx, RacingTeam.kicad_pcb, and 4 more files...
</commit_message>
<xml_diff>
--- a/RacingTeam/PCBBom.xlsx
+++ b/RacingTeam/PCBBom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayden Bourdeau\SyncedGit\RacingTeam\RacingTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216B1598-B2C7-407D-A471-616F261AD15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AEA2A0-693E-4CB3-B77A-26E0AF2C886D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
   </bookViews>
@@ -732,7 +732,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update 2N7002H6327XTSA2.kicad_mod, 4N35SM.kicad_mod, and 69 more files...
</commit_message>
<xml_diff>
--- a/RacingTeam/PCBBom.xlsx
+++ b/RacingTeam/PCBBom.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayden Bourdeau\SyncedGit\RacingTeam\RacingTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AEA2A0-693E-4CB3-B77A-26E0AF2C886D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D882156-1905-44E9-A3C6-D6B14E36646A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
+    <workbookView xWindow="0" yWindow="3795" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="BOMConfirmed" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="163">
   <si>
     <t>Item</t>
   </si>
@@ -192,9 +193,6 @@
     <t>2034-1106-ND</t>
   </si>
   <si>
-    <t>R1-R4</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0805FT249K/1760185</t>
   </si>
   <si>
@@ -210,9 +208,6 @@
     <t>Resistor for Voltage Division (1.3k) (0805)</t>
   </si>
   <si>
-    <t>R7-R9</t>
-  </si>
-  <si>
     <t>RNCP0805FTD1K30</t>
   </si>
   <si>
@@ -358,6 +353,177 @@
   </si>
   <si>
     <t>F1-F5</t>
+  </si>
+  <si>
+    <t>GLV LDO</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/TL750L12CD/373208</t>
+  </si>
+  <si>
+    <t>Q2,Q3,Q5,Q7</t>
+  </si>
+  <si>
+    <t>Q1,Q4,Q6,Q8</t>
+  </si>
+  <si>
+    <t>RSC002P03T316</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/rohm-semiconductor/RSC002P03T316/5042810</t>
+  </si>
+  <si>
+    <t>D1,D2</t>
+  </si>
+  <si>
+    <t>TS Board Connector</t>
+  </si>
+  <si>
+    <t>TSAL Light Connector</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0878340619/3303499</t>
+  </si>
+  <si>
+    <t>M4 Screws for TS Connector</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Single Pin Header (2.54mm)</t>
+  </si>
+  <si>
+    <t>J2,J3,J4,J5</t>
+  </si>
+  <si>
+    <t>Terminal Block for Relays</t>
+  </si>
+  <si>
+    <t>J6,J7,J8</t>
+  </si>
+  <si>
+    <t>TBL001-500-02GY-2GY</t>
+  </si>
+  <si>
+    <t>U1,U2</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>D3,D4,D5</t>
+  </si>
+  <si>
+    <t>EC3SAW-24S12P</t>
+  </si>
+  <si>
+    <t>PSU (HV-GLV)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/cincon-electronics-co-ltd/EC3SAW-24S12P/9682359?s=N4IgTCBcDa4AwGYAsBaAjGuA2FA5AIiALoC%2BQA</t>
+  </si>
+  <si>
+    <t>R6,R12,R13,R14</t>
+  </si>
+  <si>
+    <t>R1,R2,R3</t>
+  </si>
+  <si>
+    <t>R16,R17,R18,R19</t>
+  </si>
+  <si>
+    <t>R20,R22,R26,R27,R29</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>Resistor for CMOS Pullup (10k) (0603)</t>
+  </si>
+  <si>
+    <t>R26,R31</t>
+  </si>
+  <si>
+    <t>Resistor for LED (499Ohm) (0603)</t>
+  </si>
+  <si>
+    <t>Diagnostic LED's (Red) (0805)</t>
+  </si>
+  <si>
+    <t>R28,R32</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>R8,R9,R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>Resistor (0 Ohm) (0805)</t>
+  </si>
+  <si>
+    <t>Resistor for Voltage Division (22k) (0805)</t>
+  </si>
+  <si>
+    <t>R33,R34,R35,R36</t>
+  </si>
+  <si>
+    <t>Capacitor for Op-Amp (10nF)(0603)</t>
+  </si>
+  <si>
+    <t>C1,C3</t>
+  </si>
+  <si>
+    <t>C5,C6</t>
+  </si>
+  <si>
+    <t>Capacitor  for 555 Timer(100nF)(0603)</t>
+  </si>
+  <si>
+    <t>Capacitor for 555 Timer (1uF)(0603)</t>
+  </si>
+  <si>
+    <t>Capacitor for GLV Regulator (1uF)(0603)</t>
+  </si>
+  <si>
+    <t>C9,C10</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>GLV Regulator</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>MC78M12ABDTRKG</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/MC78M12ABDTRKG/1481457?s=N4IgTCBcDaILIGEDsAOOBGMBBAQgEQBUAlAaQHEQBdAXyA</t>
+  </si>
+  <si>
+    <t>Jumper</t>
+  </si>
+  <si>
+    <t>Shunt</t>
   </si>
 </sst>
 </file>
@@ -729,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659DCB98-9E00-43BC-A3B3-A9EBD8392DA4}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +958,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
@@ -809,7 +975,7 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -894,7 +1060,7 @@
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2">
-        <f>G8*I8</f>
+        <f t="shared" ref="K8:K16" si="0">G8*I8</f>
         <v>2.39</v>
       </c>
       <c r="L8" s="2"/>
@@ -924,7 +1090,7 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2">
-        <f t="shared" ref="K9:K25" si="0">G9*I9</f>
+        <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
       <c r="L9" s="2"/>
@@ -949,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="K10">
-        <f>G10*I10</f>
+        <f t="shared" si="0"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="M10" s="4" t="s">
@@ -978,7 +1144,7 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2">
-        <f>G11*I11</f>
+        <f t="shared" si="0"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="L11" s="2"/>
@@ -1136,77 +1302,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2">
-        <v>4</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2">
-        <v>3</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
+    <row r="18" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
@@ -1218,25 +1325,25 @@
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K19:K25" si="1">G19*I19</f>
         <v>0.6</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
@@ -1248,25 +1355,25 @@
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
@@ -1278,25 +1385,25 @@
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
@@ -1308,25 +1415,25 @@
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
@@ -1338,25 +1445,25 @@
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.02</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
@@ -1368,25 +1475,25 @@
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
@@ -1398,23 +1505,23 @@
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
@@ -1431,15 +1538,15 @@
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G27" s="2">
         <v>0.15</v>
@@ -1452,15 +1559,15 @@
         <v>0.15</v>
       </c>
       <c r="M27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" t="s">
         <v>94</v>
-      </c>
-      <c r="E28" t="s">
-        <v>96</v>
       </c>
       <c r="G28" s="2">
         <v>0.15</v>
@@ -1473,15 +1580,15 @@
         <v>0.15</v>
       </c>
       <c r="M28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G29" s="2">
         <v>0.15</v>
@@ -1494,12 +1601,12 @@
         <v>0.15</v>
       </c>
       <c r="M29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G30" s="2">
         <v>0.15</v>
@@ -1512,15 +1619,15 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="M30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G31" s="2">
         <v>4.0599999999999996</v>
@@ -1532,15 +1639,23 @@
         <f>I31*G31</f>
         <v>20.299999999999997</v>
       </c>
-      <c r="M31" t="s">
-        <v>105</v>
+      <c r="M31" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C32" t="s">
+      <c r="M33" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1561,6 +1676,832 @@
     <hyperlink ref="M9" r:id="rId13" xr:uid="{2E109D78-6982-4043-8D6D-48296465E121}"/>
     <hyperlink ref="M8" r:id="rId14" xr:uid="{D063395C-1335-4145-9AAE-EBBC5462897E}"/>
     <hyperlink ref="M5" r:id="rId15" xr:uid="{073FF774-A8B3-4EB6-865F-37A44A0EE3EF}"/>
+    <hyperlink ref="M31" r:id="rId16" xr:uid="{7807D7F8-0185-49D5-9FB7-0D8F607E88EE}"/>
+    <hyperlink ref="M33" r:id="rId17" xr:uid="{05447D7C-5759-4EBF-9195-E89612D07F8F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B983F1E2-83C6-443D-B8F3-AA40413DF129}">
+  <dimension ref="C3:O41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>0.52</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <f>K5*I5</f>
+        <v>2.08</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6">
+        <v>0.4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <f>K6*I6</f>
+        <v>1.6</v>
+      </c>
+      <c r="O6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7">
+        <v>1.02</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <f>K7*I7</f>
+        <v>2.04</v>
+      </c>
+      <c r="O7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>2.39</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f>K8*I8</f>
+        <v>2.39</v>
+      </c>
+      <c r="O8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10">
+        <v>878340619</v>
+      </c>
+      <c r="I10">
+        <v>1.93</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f>K10*I10</f>
+        <v>1.93</v>
+      </c>
+      <c r="O10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <f>K11*I11</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="O11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <f>K12*I12</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13">
+        <v>1.57</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <f>K13*I13</f>
+        <v>3.14</v>
+      </c>
+      <c r="O13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14">
+        <v>1.17</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <f>K14*I14</f>
+        <v>1.17</v>
+      </c>
+      <c r="O14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15">
+        <v>1.24</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15:M39" si="0">K15*I15</f>
+        <v>1.24</v>
+      </c>
+      <c r="O15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16">
+        <v>0.65</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="O16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>19.170000000000002</v>
+      </c>
+      <c r="O17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2">
+        <v>4</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2">
+        <v>3</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20">
+        <v>0.15</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21">
+        <v>0.15</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22">
+        <v>0.15</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2">
+        <v>2</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="N23" s="2"/>
+      <c r="O23" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24">
+        <v>0.51</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25">
+        <v>0.84</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>0.84</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26">
+        <v>0.69</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>0.69</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27" t="s">
+        <v>82</v>
+      </c>
+      <c r="I27">
+        <v>0.19</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G28" t="s">
+        <v>84</v>
+      </c>
+      <c r="I28">
+        <v>0.15</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" t="s">
+        <v>144</v>
+      </c>
+      <c r="G29" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29">
+        <v>0.15</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30">
+        <v>0.15</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="O30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>147</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>148</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="K33">
+        <v>5</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>20.299999999999997</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" t="s">
+        <v>150</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" t="s">
+        <v>151</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" t="s">
+        <v>156</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G39" t="s">
+        <v>159</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{385DC4F5-227E-4C97-80C6-85D1210EC2B4}"/>
+    <hyperlink ref="O12" r:id="rId2" xr:uid="{9B96B502-012B-487D-9727-C5D721DB2A8F}"/>
+    <hyperlink ref="O18" r:id="rId3" xr:uid="{C3CB9D94-C592-4661-AFF7-5EA98D1817D7}"/>
+    <hyperlink ref="O19" r:id="rId4" xr:uid="{CE0A6BAA-7E52-4763-8559-6D4C64253FC1}"/>
+    <hyperlink ref="O20" r:id="rId5" xr:uid="{ED07486A-4106-460B-B738-DFB6EA48570B}"/>
+    <hyperlink ref="O21" r:id="rId6" xr:uid="{6E138B40-1525-4B6F-A60E-7049C3F18892}"/>
+    <hyperlink ref="O22" r:id="rId7" xr:uid="{F35FFA69-B1FC-428D-B8EE-C44AA304E416}"/>
+    <hyperlink ref="O23" r:id="rId8" xr:uid="{0358AC0A-DBB0-4B42-924D-E391B4A60FFD}"/>
+    <hyperlink ref="O24" r:id="rId9" xr:uid="{6682EB61-418A-46CF-B63A-7D2499A9C52D}"/>
+    <hyperlink ref="O25" r:id="rId10" xr:uid="{9AAEEFB6-3E00-4270-9074-39603160548F}"/>
+    <hyperlink ref="O26" r:id="rId11" xr:uid="{C3F0BFF4-D760-4BBA-9F8E-F6915B683468}"/>
+    <hyperlink ref="O27" r:id="rId12" xr:uid="{987CD2E1-5807-41E3-987A-A08D1F90C417}"/>
+    <hyperlink ref="O28" r:id="rId13" xr:uid="{116BD188-74B0-4D06-8B65-C2A95492A735}"/>
+    <hyperlink ref="O29" r:id="rId14" xr:uid="{DFEA5051-4F03-44B5-9EF7-3CA1D89EF14B}"/>
+    <hyperlink ref="O33" r:id="rId15" xr:uid="{65096647-BD95-477C-9EA4-3830D355998E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>

<commit_message>
Update GRC22Footprints.mod, C_0603_1608Metric.step, and 19 more files...
</commit_message>
<xml_diff>
--- a/RacingTeam/PCBBom.xlsx
+++ b/RacingTeam/PCBBom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayden Bourdeau\SyncedGit\RacingTeam\RacingTeam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Synced KiCAD\RacingTeam\RacingTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D882156-1905-44E9-A3C6-D6B14E36646A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57226C5C-C36E-41ED-8649-9102D40113F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3795" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
   <si>
     <t>Item</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>Shunt</t>
+  </si>
+  <si>
+    <t>0154003.DR</t>
   </si>
 </sst>
 </file>
@@ -901,10 +904,10 @@
       <selection activeCell="A32" sqref="A32:M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -933,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -948,7 +951,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -978,7 +981,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1302,8 +1305,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>64</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>73</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>85</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>92</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>98</v>
       </c>
@@ -1622,7 +1625,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>102</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>104</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>106</v>
       </c>
@@ -1689,12 +1692,12 @@
   <dimension ref="C3:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -1767,11 +1770,11 @@
         <f>K6*I6</f>
         <v>1.6</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C8" s="2" t="s">
         <v>113</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>117</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>114</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="3:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>119</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>121</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
@@ -1991,11 +1994,11 @@
         <f t="shared" si="0"/>
         <v>1.9500000000000002</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C17" s="2" t="s">
         <v>128</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C19" s="2" t="s">
         <v>56</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>60</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>61</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>64</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C23" s="2" t="s">
         <v>135</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>137</v>
       </c>
@@ -2205,7 +2208,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>138</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>74</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>81</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>85</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
         <v>92</v>
       </c>
@@ -2325,7 +2328,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
         <v>93</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>147</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
         <v>146</v>
       </c>
@@ -2370,28 +2373,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
         <v>102</v>
       </c>
       <c r="E33" t="s">
         <v>105</v>
       </c>
-      <c r="I33">
-        <v>4.0599999999999996</v>
+      <c r="G33" t="s">
+        <v>163</v>
       </c>
       <c r="K33">
         <v>5</v>
       </c>
       <c r="M33">
         <f t="shared" si="0"/>
-        <v>20.299999999999997</v>
+        <v>0</v>
       </c>
       <c r="O33" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>104</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>149</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>152</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
         <v>153</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>154</v>
       </c>
@@ -2451,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>157</v>
       </c>
@@ -2475,12 +2478,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>162</v>
       </c>
@@ -2502,8 +2505,10 @@
     <hyperlink ref="O28" r:id="rId13" xr:uid="{116BD188-74B0-4D06-8B65-C2A95492A735}"/>
     <hyperlink ref="O29" r:id="rId14" xr:uid="{DFEA5051-4F03-44B5-9EF7-3CA1D89EF14B}"/>
     <hyperlink ref="O33" r:id="rId15" xr:uid="{65096647-BD95-477C-9EA4-3830D355998E}"/>
+    <hyperlink ref="O16" r:id="rId16" xr:uid="{68917F24-0F3A-4E0E-ADBA-CC74AB3035BC}"/>
+    <hyperlink ref="O6" r:id="rId17" xr:uid="{98EBB041-6E9E-4EF3-B81F-91F67C9F2F79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update GRC22Footprints.mod, CONV_SPBW06F-12.kicad_mod, and 43 more files...
</commit_message>
<xml_diff>
--- a/RacingTeam/PCBBom.xlsx
+++ b/RacingTeam/PCBBom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Synced KiCAD\RacingTeam\RacingTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57226C5C-C36E-41ED-8649-9102D40113F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5B2FE1-0034-465D-B7E1-A83E26BB3386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{180AA0A3-16D2-4E3F-BFEE-3038F3471594}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="165">
   <si>
     <t>Item</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t>0154003.DR</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1689,10 +1692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B983F1E2-83C6-443D-B8F3-AA40413DF129}">
-  <dimension ref="C3:O41"/>
+  <dimension ref="C3:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2486,6 +2489,15 @@
     <row r="41" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>164</v>
+      </c>
+      <c r="M42">
+        <f>SUM(M5:M41)</f>
+        <v>48.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>